<commit_message>
Distinguish tokens SERVICE_CD for compiler directives and SERVICE for TypeCobol (which is a Cobol reserved keyword anyway)
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Code elements starting tokens.xlsx
+++ b/TypeCobol/Documentation/Studies/Code elements starting tokens.xlsx
@@ -13,14 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
-    <sheet name="v2 - 11_2016" sheetId="2" r:id="rId2"/>
-    <sheet name="v2 - ambiguities" sheetId="3" r:id="rId3"/>
-    <sheet name="MultilineScanState" sheetId="4" r:id="rId4"/>
+    <sheet name="MultilineScanState" sheetId="4" r:id="rId2"/>
+    <sheet name="v2 - 11_2016" sheetId="2" r:id="rId3"/>
+    <sheet name="v2 - ambiguities" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'v1'!$E$1:$E$104</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2802,7 +2802,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2857,6 +2857,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2870,7 +2876,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2988,6 +2994,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5034,6 +5043,441 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="45"/>
+    <col min="6" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="86.7109375" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F1" s="49" t="s">
+        <v>450</v>
+      </c>
+      <c r="G1" s="48"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2" s="45"/>
+      <c r="H2" s="46"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="C4" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="G4" t="s">
+        <v>344</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="C5" s="17"/>
+      <c r="F5" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="G5" t="s">
+        <v>452</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="E6" s="45"/>
+      <c r="H6" s="46"/>
+    </row>
+    <row r="7" spans="1:8" s="23" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="E7" s="45"/>
+      <c r="G7" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>347</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="G8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="47" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9" t="s">
+        <v>349</v>
+      </c>
+      <c r="G9" t="s">
+        <v>348</v>
+      </c>
+      <c r="H9" s="47" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="17" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="E11" s="45"/>
+      <c r="G11" s="52" t="s">
+        <v>457</v>
+      </c>
+      <c r="H11" s="46"/>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C12" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="G12" t="s">
+        <v>351</v>
+      </c>
+      <c r="H12" s="47" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="E13" s="45"/>
+      <c r="H13" s="46"/>
+    </row>
+    <row r="14" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="C14" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="E14" s="45"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>357</v>
+      </c>
+      <c r="C15" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>359</v>
+      </c>
+      <c r="D16" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="E18" s="45"/>
+      <c r="H18" s="46"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="17" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="E21" s="45"/>
+      <c r="H21" s="46"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="17" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="17" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="E26" s="45"/>
+      <c r="H26" s="46"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>366</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="E28" s="45"/>
+      <c r="H28" s="46"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="17" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="E31" s="45"/>
+      <c r="H31" s="46"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="17" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="E34" s="45"/>
+      <c r="H34" s="46"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>378</v>
+      </c>
+      <c r="C35" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>380</v>
+      </c>
+      <c r="D36" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="17" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="17" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>387</v>
+      </c>
+      <c r="E42" s="45"/>
+      <c r="H42" s="46"/>
+    </row>
+    <row r="43" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="E43" s="45"/>
+      <c r="H43" s="26"/>
+    </row>
+    <row r="44" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="E44" s="45"/>
+      <c r="H44" s="26"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>388</v>
+      </c>
+      <c r="C45" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="E46" s="45"/>
+      <c r="H46" s="46"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="17" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="E49" s="45"/>
+      <c r="H49" s="46"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="17" t="s">
+        <v>396</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I135"/>
   <sheetViews>
     <sheetView topLeftCell="A124" workbookViewId="0">
@@ -7951,12 +8395,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8457,7 +8901,7 @@
       <c r="F22" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="53" t="s">
         <v>414</v>
       </c>
     </row>
@@ -8511,439 +8955,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H50"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="45"/>
-    <col min="6" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="86.7109375" style="17" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F1" s="49" t="s">
-        <v>450</v>
-      </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="2" spans="1:8" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>340</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>341</v>
-      </c>
-      <c r="E2" s="45"/>
-      <c r="H2" s="46"/>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" t="s">
-        <v>344</v>
-      </c>
-      <c r="C3" t="s">
-        <v>345</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="C4" s="17" t="s">
-        <v>346</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="G4" t="s">
-        <v>344</v>
-      </c>
-      <c r="H4" s="47" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="C5" s="17"/>
-      <c r="F5" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="G5" t="s">
-        <v>452</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>342</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>343</v>
-      </c>
-      <c r="E6" s="45"/>
-      <c r="H6" s="46"/>
-    </row>
-    <row r="7" spans="1:8" s="23" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23" t="s">
-        <v>348</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="E7" s="45"/>
-      <c r="G7" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="H7" s="51" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" t="s">
-        <v>347</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="G8" t="s">
-        <v>106</v>
-      </c>
-      <c r="H8" s="47" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>348</v>
-      </c>
-      <c r="D9" t="s">
-        <v>349</v>
-      </c>
-      <c r="G9" t="s">
-        <v>348</v>
-      </c>
-      <c r="H9" s="47" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="17" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>351</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>352</v>
-      </c>
-      <c r="E11" s="45"/>
-      <c r="G11" s="52" t="s">
-        <v>457</v>
-      </c>
-      <c r="H11" s="46"/>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="C12" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="G12" t="s">
-        <v>351</v>
-      </c>
-      <c r="H12" s="47" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>354</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>355</v>
-      </c>
-      <c r="E13" s="45"/>
-      <c r="H13" s="46"/>
-    </row>
-    <row r="14" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="C14" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="E14" s="45"/>
-      <c r="H14" s="26"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>357</v>
-      </c>
-      <c r="C15" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>359</v>
-      </c>
-      <c r="D16" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="17" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>362</v>
-      </c>
-      <c r="E18" s="45"/>
-      <c r="H18" s="46"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>365</v>
-      </c>
-      <c r="E21" s="45"/>
-      <c r="H21" s="46"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="17" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="17" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>368</v>
-      </c>
-      <c r="E26" s="45"/>
-      <c r="H26" s="46"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>366</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
-        <v>370</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>371</v>
-      </c>
-      <c r="E28" s="45"/>
-      <c r="H28" s="46"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="17" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
-        <v>224</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>374</v>
-      </c>
-      <c r="E31" s="45"/>
-      <c r="H31" s="46"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="17" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="E34" s="45"/>
-      <c r="H34" s="46"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>378</v>
-      </c>
-      <c r="C35" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>380</v>
-      </c>
-      <c r="D36" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="17" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="17" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="17" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
-        <v>386</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>387</v>
-      </c>
-      <c r="E42" s="45"/>
-      <c r="H42" s="46"/>
-    </row>
-    <row r="43" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="E43" s="45"/>
-      <c r="H43" s="26"/>
-    </row>
-    <row r="44" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="26" t="s">
-        <v>390</v>
-      </c>
-      <c r="E44" s="45"/>
-      <c r="H44" s="26"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>388</v>
-      </c>
-      <c r="C45" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
-        <v>391</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>392</v>
-      </c>
-      <c r="E46" s="45"/>
-      <c r="H46" s="46"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C48" s="17" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
-        <v>395</v>
-      </c>
-      <c r="E49" s="45"/>
-      <c r="H49" s="46"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revamped the list of tokens : all potential code element startig tokens under the same token family + added three new token types LevelNumber, SectionParagraphName, QualifiedNameSeparator
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Code elements starting tokens.xlsx
+++ b/TypeCobol/Documentation/Studies/Code elements starting tokens.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="461">
   <si>
     <t>environmentDivisionHeader</t>
   </si>
@@ -1315,70 +1315,6 @@
       </rPr>
       <t xml:space="preserve">
 libraryCopy</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SERVICE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> LABEL
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SERVICE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> RELOAD UserDefinedWord
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SERVICE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ID? IS? qualifiedTextName PeriodSeparator?</t>
     </r>
   </si>
   <si>
@@ -2743,6 +2679,76 @@
     <t>ScanKeywordOrUserDefinedWord(int startIndex)
     if(TokenUtils.COBOL_INTRINSIC_FUNCTIONS.IsMatch(tokenText))
           tokenType = TokenType.IntrinsicFunctionName;</t>
+  </si>
+  <si>
+    <t>END_EXEC</t>
+  </si>
+  <si>
+    <t>execStatementEnd</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SERVICE_CD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> LABEL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SERVICE_CD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> RELOAD UserDefinedWord
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SERVICE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ID? IS? qualifiedTextName PeriodSeparator?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2876,7 +2882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2995,6 +3001,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5061,17 +5073,17 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F1" s="49" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G1" s="48"/>
       <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>340</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>341</v>
       </c>
       <c r="E2" s="45"/>
       <c r="H2" s="46"/>
@@ -5079,52 +5091,52 @@
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C3" t="s">
         <v>344</v>
       </c>
-      <c r="C3" t="s">
-        <v>345</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H3" s="47" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="C4" s="17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="C5" s="17"/>
       <c r="F5" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="G5" t="s">
         <v>451</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="50" t="s">
         <v>452</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>342</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>343</v>
       </c>
       <c r="E6" s="45"/>
       <c r="H6" s="46"/>
@@ -5132,17 +5144,17 @@
     <row r="7" spans="1:8" s="23" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="23" t="s">
+        <v>347</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>348</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>349</v>
       </c>
       <c r="E7" s="45"/>
       <c r="G7" s="22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5150,67 +5162,67 @@
         <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G8" t="s">
         <v>106</v>
       </c>
       <c r="H8" s="47" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D9" t="s">
         <v>348</v>
       </c>
-      <c r="D9" t="s">
-        <v>349</v>
-      </c>
       <c r="G9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H9" s="47" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>351</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>352</v>
       </c>
       <c r="E11" s="45"/>
       <c r="G11" s="52" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H11" s="46"/>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H12" s="47" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="B13" s="25" t="s">
         <v>354</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>355</v>
       </c>
       <c r="E13" s="45"/>
       <c r="H13" s="46"/>
@@ -5218,30 +5230,30 @@
     <row r="14" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="C14" s="26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E14" s="45"/>
       <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
+        <v>358</v>
+      </c>
+      <c r="D16" t="s">
         <v>359</v>
-      </c>
-      <c r="D16" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C17" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -5249,19 +5261,19 @@
         <v>131</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E18" s="45"/>
       <c r="H18" s="46"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -5269,19 +5281,19 @@
         <v>97</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E21" s="45"/>
       <c r="H21" s="46"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C23" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5292,7 +5304,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C25" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -5300,25 +5312,25 @@
         <v>103</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E26" s="45"/>
       <c r="H26" s="46"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="B28" s="25" t="s">
         <v>370</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>371</v>
       </c>
       <c r="E28" s="45"/>
       <c r="H28" s="46"/>
@@ -5330,7 +5342,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C30" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -5338,7 +5350,7 @@
         <v>224</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E31" s="45"/>
       <c r="H31" s="46"/>
@@ -5350,43 +5362,43 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="B34" s="25" t="s">
         <v>376</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>377</v>
       </c>
       <c r="E34" s="45"/>
       <c r="H34" s="46"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>377</v>
+      </c>
+      <c r="C35" t="s">
         <v>378</v>
-      </c>
-      <c r="C35" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D36" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C38" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -5394,81 +5406,81 @@
         <v>99</v>
       </c>
       <c r="D39" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="B42" s="25" t="s">
         <v>386</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>387</v>
       </c>
       <c r="E42" s="45"/>
       <c r="H42" s="46"/>
     </row>
     <row r="43" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="26" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E43" s="45"/>
       <c r="H43" s="26"/>
     </row>
     <row r="44" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="26" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E44" s="45"/>
       <c r="H44" s="26"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C45" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="B46" s="25" t="s">
         <v>391</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>392</v>
       </c>
       <c r="E46" s="45"/>
       <c r="H46" s="46"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E49" s="45"/>
       <c r="H49" s="46"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C50" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -5478,10 +5490,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102:C103"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35:H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5857,7 +5869,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="20" t="s">
         <v>112</v>
       </c>
       <c r="C18" t="s">
@@ -6196,16 +6208,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>141</v>
+        <v>458</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>459</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>51</v>
+        <v>458</v>
+      </c>
+      <c r="F35" t="s">
+        <v>459</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>168</v>
@@ -6219,16 +6231,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>168</v>
@@ -6242,16 +6254,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>168</v>
@@ -6264,61 +6276,61 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>280</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="H39" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>168</v>
@@ -6332,16 +6344,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>168</v>
@@ -6355,16 +6367,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>168</v>
@@ -6378,16 +6390,16 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>168</v>
@@ -6401,16 +6413,16 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>168</v>
@@ -6424,16 +6436,16 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>168</v>
@@ -6447,16 +6459,16 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>168</v>
@@ -6470,16 +6482,16 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>168</v>
@@ -6493,16 +6505,16 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>168</v>
@@ -6516,16 +6528,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>168</v>
@@ -6539,153 +6551,153 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>27</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I50" s="1" t="s">
+      <c r="G51" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>0</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I51" s="7" t="s">
+      <c r="G52" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I52" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>280</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D53" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+      <c r="H53" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>48</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G53" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I53" s="1" t="s">
+      <c r="G54" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
+    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>78</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D55" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="G55" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="H54" s="4" t="s">
+      <c r="H55" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="C55" t="s">
-        <v>28</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>170</v>
-      </c>
+      <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C56" t="s">
         <v>28</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>28</v>
@@ -6702,23 +6714,22 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="B57" t="s">
-        <v>300</v>
+        <v>186</v>
       </c>
       <c r="C57" t="s">
-        <v>266</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="F57" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G57" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H57" s="4" t="s">
-        <v>189</v>
+      <c r="H57" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>170</v>
@@ -6729,23 +6740,34 @@
         <v>267</v>
       </c>
       <c r="B58" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C58" t="s">
-        <v>268</v>
-      </c>
-      <c r="E58" s="9"/>
+        <v>266</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>267</v>
+      </c>
       <c r="F58" s="3"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="1"/>
+      <c r="G58" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>267</v>
       </c>
+      <c r="B59" t="s">
+        <v>301</v>
+      </c>
       <c r="C59" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E59" s="9"/>
       <c r="F59" s="3"/>
@@ -6755,86 +6777,76 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="C60" t="s">
+        <v>270</v>
+      </c>
+      <c r="E60" s="9"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>12</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I60" s="7" t="s">
+      <c r="G61" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I61" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+    <row r="62" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>11</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D62" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="G62" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="H61" s="4" t="s">
+      <c r="H62" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I62" s="7" t="s">
-        <v>238</v>
-      </c>
+      <c r="I62" s="1"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C63" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>168</v>
@@ -6842,22 +6854,22 @@
       <c r="H63" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I63" s="1" t="s">
-        <v>170</v>
+      <c r="I63" s="7" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C64" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>168</v>
@@ -6871,81 +6883,88 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" t="s">
+        <v>29</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F66" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G65" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I65" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="B66" t="s">
-        <v>306</v>
-      </c>
-      <c r="C66" t="s">
-        <v>216</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="G66" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H66" s="4" t="s">
-        <v>196</v>
+      <c r="H66" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>244</v>
       </c>
       <c r="B67" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C67" t="s">
-        <v>251</v>
-      </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="7"/>
+        <v>216</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>244</v>
       </c>
       <c r="B68" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C68" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -6958,10 +6977,10 @@
         <v>244</v>
       </c>
       <c r="B69" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C69" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -6971,13 +6990,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B70" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C70" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -6985,57 +7004,57 @@
       <c r="H70" s="4"/>
       <c r="I70" s="7"/>
     </row>
-    <row r="71" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A71" s="18" t="s">
-        <v>243</v>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
+        <v>253</v>
       </c>
       <c r="B71" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C71" t="s">
-        <v>216</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="I71" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="7"/>
+    </row>
+    <row r="72" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>243</v>
       </c>
       <c r="B72" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="C72" t="s">
-        <v>251</v>
-      </c>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="7"/>
+        <v>216</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
         <v>243</v>
       </c>
       <c r="B73" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C73" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -7048,10 +7067,10 @@
         <v>243</v>
       </c>
       <c r="B74" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C74" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -7064,10 +7083,10 @@
         <v>243</v>
       </c>
       <c r="B75" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C75" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -7077,39 +7096,32 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>138</v>
+        <v>243</v>
+      </c>
+      <c r="B76" t="s">
+        <v>303</v>
       </c>
       <c r="C76" t="s">
-        <v>50</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>170</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="7"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="C77" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>168</v>
@@ -7123,16 +7135,16 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>168</v>
@@ -7140,136 +7152,136 @@
       <c r="H78" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I78" s="7" t="s">
-        <v>238</v>
+      <c r="I78" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C79" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>32</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E80" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G79" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I79" s="1" t="s">
+      <c r="G80" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I80" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
+    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>80</v>
       </c>
-      <c r="D80" s="10" t="s">
+      <c r="D81" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G80" s="4" t="s">
+      <c r="G81" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="H81" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="I80" s="1"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>52</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G81" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I81" s="1" t="s">
+      <c r="G82" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I82" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>13</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="F83" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H83" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="I82" s="1"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C83" t="s">
-        <v>16</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I83" s="7" t="s">
-        <v>238</v>
-      </c>
+      <c r="I83" s="1"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C84" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>168</v>
@@ -7283,16 +7295,16 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C85" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>168</v>
@@ -7300,22 +7312,22 @@
       <c r="H85" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I85" s="1" t="s">
-        <v>170</v>
+      <c r="I85" s="7" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C86" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>168</v>
@@ -7329,16 +7341,16 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
-        <v>226</v>
+        <v>119</v>
       </c>
       <c r="C87" t="s">
-        <v>245</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>226</v>
+        <v>34</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>227</v>
+        <v>34</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>168</v>
@@ -7346,109 +7358,116 @@
       <c r="H87" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I87" s="7" t="s">
-        <v>238</v>
+      <c r="I87" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="C88" t="s">
+        <v>245</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>54</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E89" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="F89" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G88" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I88" s="1" t="s">
+      <c r="G89" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I89" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
+    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>85</v>
       </c>
-      <c r="D89" s="10" t="s">
+      <c r="D90" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E90" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F89" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G89" s="4" t="s">
+      <c r="G90" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H89" s="4" t="s">
+      <c r="H90" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="I89" s="1"/>
-    </row>
-    <row r="90" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="B90" t="s">
-        <v>310</v>
-      </c>
-      <c r="C90" t="s">
-        <v>278</v>
-      </c>
-      <c r="D90" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G90" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="H90" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="B91" s="10" t="s">
-        <v>312</v>
+      <c r="B91" t="s">
+        <v>310</v>
       </c>
       <c r="C91" t="s">
-        <v>281</v>
-      </c>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
+        <v>278</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>202</v>
+      </c>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="B92" t="s">
-        <v>132</v>
+      <c r="B92" s="10" t="s">
+        <v>312</v>
       </c>
       <c r="C92" t="s">
-        <v>81</v>
+        <v>281</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
@@ -7461,10 +7480,10 @@
         <v>279</v>
       </c>
       <c r="B93" t="s">
-        <v>309</v>
+        <v>132</v>
       </c>
       <c r="C93" t="s">
-        <v>283</v>
+        <v>81</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
@@ -7477,10 +7496,10 @@
         <v>279</v>
       </c>
       <c r="B94" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C94" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
@@ -7493,10 +7512,10 @@
         <v>279</v>
       </c>
       <c r="B95" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C95" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
@@ -7505,69 +7524,69 @@
       <c r="I95" s="1"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="18" t="s">
+      <c r="A96" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="B96" t="s">
+        <v>308</v>
+      </c>
+      <c r="C96" t="s">
+        <v>285</v>
+      </c>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>3</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="F97" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G96" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I96" s="7" t="s">
+      <c r="G97" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I97" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="255" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="B97" t="s">
-        <v>204</v>
-      </c>
-      <c r="C97" t="s">
-        <v>78</v>
-      </c>
-      <c r="D97" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="G97" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="H97" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="I97" s="1"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
         <v>282</v>
       </c>
       <c r="B98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C98" t="s">
-        <v>79</v>
-      </c>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="I98" s="1"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -7575,10 +7594,10 @@
         <v>282</v>
       </c>
       <c r="B99" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C99" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -7587,198 +7606,191 @@
       <c r="I99" s="1"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="18" t="s">
+      <c r="A100" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="B100" t="s">
+        <v>213</v>
+      </c>
+      <c r="C100" t="s">
+        <v>77</v>
+      </c>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>35</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F100" s="1" t="s">
+      <c r="F101" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G100" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I100" s="1" t="s">
+      <c r="G101" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I101" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="C101" t="s">
-        <v>79</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G101" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H101" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="I101" s="1"/>
     </row>
     <row r="102" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C102" t="s">
+        <v>79</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>106</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>247</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="E103" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="F102" s="3" t="s">
+      <c r="F103" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="G103" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="H103" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="I102" s="1"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="17" t="s">
+      <c r="I103" s="1"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>314</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>246</v>
       </c>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="1"/>
-    </row>
-    <row r="104" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A104" s="18" t="s">
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="1"/>
+    </row>
+    <row r="105" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A105" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>271</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E105" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="F104" s="9" t="s">
+      <c r="F105" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="G104" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H104" s="4" t="s">
+      <c r="G105" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H105" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="I104" s="1" t="s">
+      <c r="I105" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="17" t="s">
+    <row r="106" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>18</v>
       </c>
-      <c r="D105" s="10" t="s">
+      <c r="D106" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="E106" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F105" s="1" t="s">
+      <c r="F106" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G105" s="2" t="s">
+      <c r="G106" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="H105" s="4" t="s">
+      <c r="H106" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="I105" s="1"/>
-    </row>
-    <row r="106" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
+      <c r="I106" s="1"/>
+    </row>
+    <row r="107" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A107" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>20</v>
       </c>
-      <c r="D106" s="10" t="s">
+      <c r="D107" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="E107" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F106" s="1" t="s">
+      <c r="F107" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G106" s="4" t="s">
+      <c r="G107" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="H106" s="2" t="s">
+      <c r="H107" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="I106" s="1"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C107" t="s">
-        <v>57</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H107" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I107" s="1" t="s">
-        <v>170</v>
-      </c>
+      <c r="I107" s="1"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="C108" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>168</v>
@@ -7792,16 +7804,16 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C109" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>168</v>
@@ -7809,22 +7821,22 @@
       <c r="H109" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I109" s="7" t="s">
-        <v>238</v>
+      <c r="I109" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>222</v>
+        <v>92</v>
       </c>
       <c r="C110" t="s">
-        <v>245</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>222</v>
+        <v>5</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>223</v>
+        <v>5</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>168</v>
@@ -7838,16 +7850,16 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
-        <v>149</v>
+        <v>222</v>
       </c>
       <c r="C111" t="s">
-        <v>59</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>149</v>
+        <v>245</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>168</v>
@@ -7855,22 +7867,22 @@
       <c r="H111" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I111" s="1" t="s">
-        <v>170</v>
+      <c r="I111" s="7" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C112" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>168</v>
@@ -7884,16 +7896,16 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
-        <v>224</v>
+        <v>151</v>
       </c>
       <c r="C113" t="s">
-        <v>245</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>224</v>
+        <v>61</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>225</v>
+        <v>61</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>168</v>
@@ -7901,22 +7913,22 @@
       <c r="H113" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I113" s="7" t="s">
-        <v>238</v>
+      <c r="I113" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="C114" t="s">
-        <v>12</v>
+        <v>245</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>12</v>
+        <v>225</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>168</v>
@@ -7930,16 +7942,16 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="C115" t="s">
-        <v>63</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>95</v>
+        <v>12</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>168</v>
@@ -7953,148 +7965,148 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C116" t="s">
+        <v>63</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C116" t="s">
+      <c r="F116" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E116" s="1" t="s">
+      <c r="G116" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I116" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="F117" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G116" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I116" s="1" t="s">
+      <c r="G117" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I117" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="117" spans="1:9" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="20" t="s">
+    <row r="118" spans="1:9" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="C117" s="13" t="s">
+      <c r="C118" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="D117" s="21" t="s">
+      <c r="D118" s="21" t="s">
         <v>335</v>
       </c>
-      <c r="E117" s="14"/>
-      <c r="F117" s="14"/>
-      <c r="G117" s="15"/>
-      <c r="H117" s="15"/>
-      <c r="I117" s="14"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="18" t="s">
+      <c r="E118" s="14"/>
+      <c r="F118" s="14"/>
+      <c r="G118" s="15"/>
+      <c r="H118" s="15"/>
+      <c r="I118" s="14"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" t="s">
         <v>37</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F118" s="1" t="s">
+      <c r="F119" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G118" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I118" s="1" t="s">
+      <c r="G119" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I119" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
+    <row r="120" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A120" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" t="s">
         <v>77</v>
       </c>
-      <c r="D119" s="10" t="s">
+      <c r="D120" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="E119" s="3" t="s">
+      <c r="E120" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="F119" s="1" t="s">
+      <c r="F120" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G119" s="4" t="s">
+      <c r="G120" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="H119" s="4" t="s">
+      <c r="H120" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="I119" s="1"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="18" t="s">
+      <c r="I120" s="1"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C121" t="s">
         <v>38</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="E121" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F120" s="1" t="s">
+      <c r="F121" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G120" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H120" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I120" s="1" t="s">
+      <c r="G121" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I121" s="1" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C121" t="s">
-        <v>2</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G121" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H121" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I121" s="7" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C122" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>168</v>
@@ -8108,16 +8120,16 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="18" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="C123" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>155</v>
+        <v>91</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>168</v>
@@ -8125,22 +8137,22 @@
       <c r="H123" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I123" s="1" t="s">
-        <v>170</v>
+      <c r="I123" s="7" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="18" t="s">
-        <v>269</v>
+        <v>155</v>
       </c>
       <c r="C124" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>168</v>
@@ -8154,16 +8166,16 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="18" t="s">
-        <v>157</v>
+        <v>269</v>
       </c>
       <c r="C125" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>168</v>
@@ -8177,16 +8189,16 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C126" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>168</v>
@@ -8200,16 +8212,16 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C127" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>168</v>
@@ -8223,55 +8235,51 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C128" t="s">
+        <v>71</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C129" t="s">
         <v>76</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="E129" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="F129" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G128" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I128" s="7" t="s">
+      <c r="G129" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I129" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A129" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="B129" t="s">
-        <v>230</v>
-      </c>
-      <c r="C129" t="s">
-        <v>261</v>
-      </c>
-      <c r="D129" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="F129" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="G129" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="H129" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="I129" s="1"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A130" s="17" t="s">
         <v>262</v>
       </c>
@@ -8279,12 +8287,23 @@
         <v>230</v>
       </c>
       <c r="C130" t="s">
-        <v>263</v>
-      </c>
-      <c r="E130" s="3"/>
-      <c r="F130" s="3"/>
-      <c r="G130" s="4"/>
-      <c r="H130" s="4"/>
+        <v>261</v>
+      </c>
+      <c r="D130" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="H130" s="4" t="s">
+        <v>242</v>
+      </c>
       <c r="I130" s="1"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -8292,10 +8311,10 @@
         <v>262</v>
       </c>
       <c r="B131" t="s">
-        <v>317</v>
+        <v>230</v>
       </c>
       <c r="C131" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E131" s="3"/>
       <c r="F131" s="3"/>
@@ -8304,85 +8323,101 @@
       <c r="I131" s="1"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="18" t="s">
-        <v>100</v>
+      <c r="A132" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="B132" t="s">
+        <v>317</v>
       </c>
       <c r="C132" t="s">
-        <v>14</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G132" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H132" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I132" s="7" t="s">
-        <v>238</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="1"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C133" t="s">
+        <v>14</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I133" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C134" t="s">
         <v>73</v>
       </c>
-      <c r="E133" s="1" t="s">
+      <c r="E134" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F133" s="1" t="s">
+      <c r="F134" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G133" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H133" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I133" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="B134" t="s">
-        <v>318</v>
-      </c>
-      <c r="C134" t="s">
-        <v>275</v>
-      </c>
-      <c r="E134" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F134" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="G134" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H134" s="4" t="s">
-        <v>237</v>
+      <c r="H134" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="I134" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="18" t="s">
         <v>276</v>
       </c>
       <c r="B135" t="s">
+        <v>318</v>
+      </c>
+      <c r="C135" t="s">
+        <v>275</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H135" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="B136" t="s">
         <v>319</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>165</v>
       </c>
     </row>
@@ -8399,8 +8434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8417,30 +8452,30 @@
   <sheetData>
     <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="27" t="s">
         <v>399</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>400</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>401</v>
-      </c>
       <c r="F1" s="28" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="39"/>
@@ -8450,22 +8485,22 @@
         <v>277</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C3" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>403</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>404</v>
-      </c>
       <c r="E3" s="32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -8473,22 +8508,22 @@
         <v>97</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="G4" s="30" t="s">
         <v>413</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -8499,22 +8534,22 @@
         <v>322</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>420</v>
-      </c>
       <c r="G5" s="30" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.25">
@@ -8525,19 +8560,19 @@
         <v>323</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="G6" s="30" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8548,19 +8583,19 @@
         <v>324</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8571,19 +8606,19 @@
         <v>324</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -8594,19 +8629,19 @@
         <v>325</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -8617,19 +8652,19 @@
         <v>326</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>314</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -8640,19 +8675,19 @@
         <v>327</v>
       </c>
       <c r="C11" s="22" t="s">
+        <v>429</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="D11" s="22" t="s">
-        <v>412</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="G11" s="30" t="s">
         <v>413</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="G11" s="30" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8663,19 +8698,19 @@
         <v>328</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F12" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -8683,22 +8718,22 @@
         <v>307</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>435</v>
-      </c>
       <c r="G13" s="30" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -8709,19 +8744,19 @@
         <v>329</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>438</v>
-      </c>
       <c r="G14" s="30" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="44" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -8732,19 +8767,19 @@
         <v>330</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F15" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="44" customFormat="1" ht="240" x14ac:dyDescent="0.25">
@@ -8752,22 +8787,22 @@
         <v>282</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F16" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G16" s="43" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8778,19 +8813,19 @@
         <v>332</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G17" s="43" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -8801,19 +8836,19 @@
         <v>247</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>440</v>
       </c>
-      <c r="D18" s="22" t="s">
-        <v>441</v>
-      </c>
       <c r="E18" s="22" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -8824,39 +8859,40 @@
         <v>246</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D19" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="44" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="41" t="s">
         <v>441</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>412</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="G19" s="30" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" s="10" t="s">
+      <c r="C20" s="41" t="s">
         <v>442</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>412</v>
-      </c>
-      <c r="G20" s="30" t="s">
-        <v>408</v>
+      <c r="D20" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="F20" s="54"/>
+      <c r="G20" s="55" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -8867,19 +8903,19 @@
         <v>334</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -8890,19 +8926,19 @@
         <v>338</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>339</v>
+        <v>460</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E22" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>446</v>
-      </c>
       <c r="G22" s="53" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="44" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -8913,19 +8949,19 @@
         <v>336</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G23" s="43" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -8936,19 +8972,19 @@
         <v>337</v>
       </c>
       <c r="C24" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>448</v>
-      </c>
       <c r="G24" s="30" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementation of all tokens context sensitivity (outside of the 3 new token types)
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/Code elements starting tokens.xlsx
+++ b/TypeCobol/Documentation/Studies/Code elements starting tokens.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="460">
   <si>
     <t>environmentDivisionHeader</t>
   </si>
@@ -2225,10 +2225,6 @@
       </rPr>
       <t xml:space="preserve"> DIVISION PeriodSeparator</t>
     </r>
-  </si>
-  <si>
-    <t>Not starting when :
-- previous = SERVICE</t>
   </si>
   <si>
     <t>dataDescriptionEntry
@@ -5073,7 +5069,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F1" s="49" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G1" s="48"/>
       <c r="H1" s="20"/>
@@ -5100,7 +5096,7 @@
         <v>339</v>
       </c>
       <c r="H3" s="47" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5115,20 +5111,20 @@
         <v>343</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="C5" s="17"/>
       <c r="F5" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="G5" t="s">
         <v>450</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="50" t="s">
         <v>451</v>
-      </c>
-      <c r="H5" s="50" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -5154,7 +5150,7 @@
         <v>341</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5171,7 +5167,7 @@
         <v>106</v>
       </c>
       <c r="H8" s="47" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5185,7 +5181,7 @@
         <v>347</v>
       </c>
       <c r="H9" s="47" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5202,7 +5198,7 @@
       </c>
       <c r="E11" s="45"/>
       <c r="G11" s="52" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H11" s="46"/>
     </row>
@@ -5214,7 +5210,7 @@
         <v>350</v>
       </c>
       <c r="H12" s="47" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6208,16 +6204,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="C35" t="s">
         <v>458</v>
       </c>
-      <c r="C35" t="s">
-        <v>459</v>
-      </c>
       <c r="E35" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F35" t="s">
         <v>458</v>
-      </c>
-      <c r="F35" t="s">
-        <v>459</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>168</v>
@@ -8434,8 +8430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8684,7 +8680,7 @@
         <v>412</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>413</v>
@@ -8718,19 +8714,19 @@
         <v>307</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>432</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>433</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>411</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G13" s="30" t="s">
         <v>413</v>
@@ -8744,16 +8740,16 @@
         <v>329</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>411</v>
       </c>
       <c r="E14" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>436</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>437</v>
       </c>
       <c r="G14" s="30" t="s">
         <v>413</v>
@@ -8836,16 +8832,16 @@
         <v>247</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>439</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>440</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>411</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G18" s="30" t="s">
         <v>413</v>
@@ -8859,16 +8855,16 @@
         <v>246</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E19" s="22" t="s">
         <v>411</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G19" s="30" t="s">
         <v>413</v>
@@ -8879,10 +8875,10 @@
         <v>106</v>
       </c>
       <c r="B20" s="41" t="s">
+        <v>440</v>
+      </c>
+      <c r="C20" s="41" t="s">
         <v>441</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>442</v>
       </c>
       <c r="D20" s="41" t="s">
         <v>411</v>
@@ -8903,7 +8899,7 @@
         <v>334</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>411</v>
@@ -8926,16 +8922,16 @@
         <v>338</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>411</v>
       </c>
       <c r="E22" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>444</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>445</v>
       </c>
       <c r="G22" s="53" t="s">
         <v>413</v>
@@ -8972,7 +8968,7 @@
         <v>337</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>411</v>
@@ -8981,7 +8977,7 @@
         <v>411</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G24" s="30" t="s">
         <v>413</v>

</xml_diff>